<commit_message>
Excel, Fin Econ, A2. Markowitz Efficient Frontier.
</commit_message>
<xml_diff>
--- a/A1, Isaac Aktam, 998986575.xlsx
+++ b/A1, Isaac Aktam, 998986575.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3795" windowHeight="2760" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3795" windowHeight="2760" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="JPM Hist" sheetId="14" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">JPM!$C$3:$C$121</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Portfolio!$I$2:$I$120</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -232,7 +232,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -773,7 +773,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -932,27 +932,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -995,9 +974,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1007,46 +1006,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
-    </tableStyle>
-  </tableStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1059,7 +1025,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1433,11 +1399,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-79AF-4ABD-9E57-3723656CB2E9}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1538,7 +1499,7 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1567,6 +1528,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1906,11 +1868,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4CF4-494F-A160-D6F89AF0340D}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1947,6 +1904,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1983,6 +1941,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1996,6 +1955,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2011,7 +1971,7 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2047,6 +2007,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2452,11 +2413,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C68F-4A45-AD1A-2C512B258068}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2501,6 +2457,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2612,6 +2569,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2713,7 +2671,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2749,6 +2707,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3150,11 +3109,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6F21-4452-8A0E-0808BC3A77F0}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3199,6 +3153,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3310,6 +3265,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3414,7 +3370,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3740,11 +3696,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9CE4-4F54-80B8-9ED8A5428583}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3845,7 +3796,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3881,6 +3832,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4234,11 +4186,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DD0B-4C1C-9BBA-1EB761D24401}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4283,6 +4230,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4394,6 +4342,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4498,7 +4447,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4770,11 +4719,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-82C3-476F-ADDF-82E2D3F2F03A}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4875,7 +4819,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4911,6 +4855,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5210,11 +5155,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6656-4B4D-AD37-E6E292E74A38}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5259,6 +5199,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5370,6 +5311,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5474,7 +5416,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5824,11 +5766,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-375C-4AF8-9EC1-D5CF2BB1448C}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5929,7 +5866,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5965,6 +5902,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6342,11 +6280,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C386-450C-98C7-6108659FB51E}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -6391,6 +6324,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6502,6 +6436,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6606,7 +6541,7 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6740,11 +6675,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AB8C-45E9-9821-5C7A5BC5F205}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -9860,23 +9790,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -9912,23 +9825,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -10526,7 +10422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -10962,8 +10858,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:U132"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" topLeftCell="G16" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11033,11 +10929,11 @@
       <c r="Q1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="S1" s="126" t="s">
+      <c r="S1" s="125" t="s">
         <v>62</v>
       </c>
-      <c r="T1" s="127"/>
-      <c r="U1" s="128"/>
+      <c r="T1" s="126"/>
+      <c r="U1" s="127"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
@@ -11097,10 +10993,10 @@
       <c r="S2" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="T2" s="108">
+      <c r="T2" s="123">
         <v>0.13897000000000001</v>
       </c>
-      <c r="U2" s="109"/>
+      <c r="U2" s="124"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
@@ -11149,13 +11045,13 @@
       <c r="N3" s="63">
         <v>0.25</v>
       </c>
-      <c r="S3" s="101" t="s">
+      <c r="S3" s="116" t="s">
         <v>56</v>
       </c>
-      <c r="T3" s="102">
+      <c r="T3" s="117">
         <v>8.6516999999999997E-2</v>
       </c>
-      <c r="U3" s="103">
+      <c r="U3" s="118">
         <f>N2*T3</f>
         <v>2.1629249999999999E-2</v>
       </c>
@@ -11213,13 +11109,13 @@
       <c r="Q4" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="S4" s="104" t="s">
+      <c r="S4" s="119" t="s">
         <v>57</v>
       </c>
       <c r="T4" s="52">
         <v>7.2039000000000006E-2</v>
       </c>
-      <c r="U4" s="105">
+      <c r="U4" s="120">
         <f t="shared" ref="U4:U6" si="6">N3*T4</f>
         <v>1.8009750000000001E-2</v>
       </c>
@@ -11278,13 +11174,13 @@
         <f>(30/118)</f>
         <v>0.25423728813559321</v>
       </c>
-      <c r="S5" s="104" t="s">
+      <c r="S5" s="119" t="s">
         <v>58</v>
       </c>
       <c r="T5" s="52">
         <v>5.4690913000000001E-2</v>
       </c>
-      <c r="U5" s="105">
+      <c r="U5" s="120">
         <f t="shared" si="6"/>
         <v>1.367272825E-2</v>
       </c>
@@ -11330,13 +11226,13 @@
         <v>-0.05</v>
       </c>
       <c r="L6" s="52"/>
-      <c r="S6" s="104" t="s">
+      <c r="S6" s="119" t="s">
         <v>59</v>
       </c>
       <c r="T6" s="52">
         <v>8.1641000000000005E-2</v>
       </c>
-      <c r="U6" s="105">
+      <c r="U6" s="120">
         <f t="shared" si="6"/>
         <v>2.0410250000000001E-2</v>
       </c>
@@ -11370,7 +11266,7 @@
         <f t="shared" si="3"/>
         <v>-1.1023549322716765E-2</v>
       </c>
-      <c r="I7" s="110">
+      <c r="I7" s="128">
         <f t="shared" si="4"/>
         <v>2.0956819825986461E-2</v>
       </c>
@@ -11384,8 +11280,8 @@
       <c r="S7" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="T7" s="106"/>
-      <c r="U7" s="107">
+      <c r="T7" s="121"/>
+      <c r="U7" s="122">
         <f>SUM(U3:U6)</f>
         <v>7.372197825E-2</v>
       </c>
@@ -11437,18 +11333,18 @@
       <c r="N8" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="P8" s="116" t="s">
+      <c r="P8" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="Q8" s="117"/>
+      <c r="Q8" s="102"/>
       <c r="S8" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="T8" s="106">
+      <c r="T8" s="121">
         <f>T2-U7</f>
         <v>6.524802175000001E-2</v>
       </c>
-      <c r="U8" s="107"/>
+      <c r="U8" s="122"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
@@ -11502,10 +11398,10 @@
       <c r="P9" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="Q9" s="97" t="s">
+      <c r="Q9" s="111" t="s">
         <v>40</v>
       </c>
-      <c r="S9" s="96"/>
+      <c r="S9" s="110"/>
       <c r="T9" s="52"/>
       <c r="U9" s="52"/>
     </row>
@@ -11558,7 +11454,7 @@
         <f>NORMDIST(0,M9,M12,TRUE)</f>
         <v>0.15416716519532667</v>
       </c>
-      <c r="S10" s="96"/>
+      <c r="S10" s="110"/>
       <c r="T10" s="52"/>
       <c r="U10" s="52"/>
     </row>
@@ -11639,7 +11535,7 @@
         <f t="shared" si="3"/>
         <v>5.1915571497526975E-3</v>
       </c>
-      <c r="I12" s="110">
+      <c r="I12" s="128">
         <f t="shared" si="4"/>
         <v>4.721043512512807E-2</v>
       </c>
@@ -16037,14 +15933,14 @@
       <c r="S120"/>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A122" s="96"/>
-      <c r="B122" s="96"/>
-      <c r="C122" s="96"/>
-      <c r="F122" s="125"/>
-      <c r="G122" s="125"/>
-      <c r="H122" s="125"/>
-      <c r="I122" s="125"/>
-      <c r="J122" s="125"/>
+      <c r="A122" s="110"/>
+      <c r="B122" s="110"/>
+      <c r="C122" s="110"/>
+      <c r="F122" s="112"/>
+      <c r="G122" s="112"/>
+      <c r="H122" s="112"/>
+      <c r="I122" s="112"/>
+      <c r="J122" s="112"/>
       <c r="K122" s="52"/>
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.25">
@@ -16052,11 +15948,11 @@
       <c r="B123" s="52"/>
       <c r="C123" s="52"/>
       <c r="F123" s="52"/>
-      <c r="G123" s="98"/>
-      <c r="H123" s="98"/>
-      <c r="I123" s="98"/>
-      <c r="J123" s="98"/>
-      <c r="K123" s="99"/>
+      <c r="G123" s="113"/>
+      <c r="H123" s="113"/>
+      <c r="I123" s="113"/>
+      <c r="J123" s="113"/>
+      <c r="K123" s="114"/>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" s="52"/>
@@ -16067,7 +15963,7 @@
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
-      <c r="K124" s="100"/>
+      <c r="K124" s="115"/>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" s="52"/>
@@ -16078,7 +15974,7 @@
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
-      <c r="K125" s="100"/>
+      <c r="K125" s="115"/>
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" s="52"/>
@@ -16089,7 +15985,7 @@
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
-      <c r="K126" s="100"/>
+      <c r="K126" s="115"/>
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F127" s="3"/>
@@ -16097,15 +15993,15 @@
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
       <c r="J127" s="3"/>
-      <c r="K127" s="100"/>
+      <c r="K127" s="115"/>
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F128" s="52"/>
       <c r="G128" s="52"/>
       <c r="H128" s="52"/>
-      <c r="I128" s="98"/>
+      <c r="I128" s="113"/>
       <c r="J128" s="52"/>
-      <c r="K128" s="100"/>
+      <c r="K128" s="115"/>
     </row>
     <row r="129" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G129" s="3"/>
@@ -16156,7 +16052,7 @@
   <dimension ref="A1:L122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A122"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16173,27 +16069,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="113" t="s">
+      <c r="B1" s="98"/>
+      <c r="C1" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="113"/>
+      <c r="D1" s="98"/>
       <c r="E1" s="79" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="33"/>
-      <c r="G1" s="111" t="s">
+      <c r="G1" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="112"/>
+      <c r="H1" s="97"/>
       <c r="I1" s="33"/>
-      <c r="J1" s="111" t="s">
+      <c r="J1" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="112"/>
+      <c r="K1" s="97"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="93" t="s">
@@ -16248,8 +16144,8 @@
         <v>1.0117705472098169E-2</v>
       </c>
       <c r="H3" s="24">
-        <f>GEOMEAN(ABS(C3:C118))</f>
-        <v>9.7481610815391834E-3</v>
+        <f>-1+GEOMEAN(L3:L121)</f>
+        <v>4.7983474974307327E-2</v>
       </c>
       <c r="J3" s="24">
         <f>MIN(C3:C121)</f>
@@ -16260,9 +16156,9 @@
         <v>0.24374492962980396</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="82">
-        <v>42339</v>
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42310</v>
       </c>
       <c r="B4">
         <v>66.235671999999994</v>
@@ -16279,9 +16175,9 @@
         <v>-0.24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="82">
-        <v>42339</v>
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42278</v>
       </c>
       <c r="B5">
         <v>63.821860999999998</v>
@@ -16299,8 +16195,8 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="82">
-        <v>42339</v>
+      <c r="A6" s="83">
+        <v>42248</v>
       </c>
       <c r="B6" s="25">
         <v>60.129852</v>
@@ -16317,9 +16213,9 @@
         <v>-0.22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="82">
-        <v>42339</v>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="83">
+        <v>42219</v>
       </c>
       <c r="B7" s="25">
         <v>63.216721</v>
@@ -16341,14 +16237,14 @@
       <c r="H7" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="J7" s="114" t="s">
+      <c r="J7" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="K7" s="115"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="82">
-        <v>42339</v>
+      <c r="K7" s="100"/>
+    </row>
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>42186</v>
       </c>
       <c r="B8">
         <v>67.585678000000001</v>
@@ -16365,9 +16261,9 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="82">
-        <v>42339</v>
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>42156</v>
       </c>
       <c r="B9">
         <v>66.392348999999996</v>
@@ -16384,9 +16280,9 @@
         <v>-0.19</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="82">
-        <v>42339</v>
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>42125</v>
       </c>
       <c r="B10">
         <v>64.452309</v>
@@ -16403,9 +16299,9 @@
         <v>-0.18</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="82">
-        <v>42339</v>
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>42095</v>
       </c>
       <c r="B11">
         <v>61.983173000000001</v>
@@ -16423,8 +16319,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="82">
-        <v>42339</v>
+      <c r="A12" s="83">
+        <v>42065</v>
       </c>
       <c r="B12" s="25">
         <v>58.965347000000001</v>
@@ -16456,8 +16352,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="82">
-        <v>42339</v>
+      <c r="A13" s="83">
+        <v>42037</v>
       </c>
       <c r="B13" s="25">
         <v>59.646687</v>
@@ -16475,7 +16371,7 @@
       </c>
       <c r="J13" s="91">
         <f>_xlfn.NORM.DIST(0,H3,G12,TRUE)</f>
-        <v>0.45514480665460122</v>
+        <v>0.28957980340836653</v>
       </c>
       <c r="K13" s="24">
         <f>_xlfn.NORM.DIST(0,G3,G12,TRUE)</f>
@@ -16483,8 +16379,8 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="82">
-        <v>42339</v>
+      <c r="A14" s="83">
+        <v>42006</v>
       </c>
       <c r="B14" s="25">
         <v>52.930594999999997</v>
@@ -16501,9 +16397,9 @@
         <v>-0.14000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="82">
-        <v>42339</v>
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>41974</v>
       </c>
       <c r="B15">
         <v>60.522697000000001</v>
@@ -16520,9 +16416,9 @@
         <v>-0.13</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="82">
-        <v>42339</v>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="83">
+        <v>41946</v>
       </c>
       <c r="B16" s="25">
         <v>58.182254999999998</v>
@@ -16539,9 +16435,9 @@
         <v>-0.12</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="82">
-        <v>42339</v>
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>41913</v>
       </c>
       <c r="B17">
         <v>58.491734000000001</v>
@@ -16558,9 +16454,9 @@
         <v>-0.11</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="82">
-        <v>42339</v>
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>41884</v>
       </c>
       <c r="B18">
         <v>57.869736000000003</v>
@@ -16577,9 +16473,9 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="82">
-        <v>42339</v>
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>41852</v>
       </c>
       <c r="B19">
         <v>57.110816999999997</v>
@@ -16596,9 +16492,9 @@
         <v>-0.09</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="82">
-        <v>42339</v>
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>41821</v>
       </c>
       <c r="B20">
         <v>55.400852</v>
@@ -16615,9 +16511,9 @@
         <v>-0.08</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="82">
-        <v>42339</v>
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>41792</v>
       </c>
       <c r="B21">
         <v>54.968563000000003</v>
@@ -16635,8 +16531,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="82">
-        <v>42339</v>
+      <c r="A22" s="83">
+        <v>41760</v>
       </c>
       <c r="B22" s="25">
         <v>53.012894000000003</v>
@@ -16654,8 +16550,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="82">
-        <v>42339</v>
+      <c r="A23" s="83">
+        <v>41730</v>
       </c>
       <c r="B23" s="25">
         <v>53.404029999999999</v>
@@ -16672,7 +16568,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>41701</v>
       </c>
@@ -16691,7 +16587,7 @@
         <v>-0.04</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>41673</v>
       </c>
@@ -16711,8 +16607,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="82">
-        <v>42339</v>
+      <c r="A26" s="83">
+        <v>41641</v>
       </c>
       <c r="B26" s="25">
         <v>52.481772999999997</v>
@@ -16729,7 +16625,7 @@
         <v>-0.02</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>41610</v>
       </c>
@@ -16748,7 +16644,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>41579</v>
       </c>
@@ -16767,7 +16663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>41548</v>
       </c>
@@ -16786,7 +16682,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>41520</v>
       </c>
@@ -16806,8 +16702,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="82">
-        <v>42339</v>
+      <c r="A31" s="83">
+        <v>41487</v>
       </c>
       <c r="B31" s="25">
         <v>47.243564999999997</v>
@@ -16824,7 +16720,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>41456</v>
       </c>
@@ -16844,8 +16740,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="82">
-        <v>42339</v>
+      <c r="A33" s="83">
+        <v>41428</v>
       </c>
       <c r="B33" s="25">
         <v>48.99926</v>
@@ -16862,7 +16758,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>41395</v>
       </c>
@@ -16881,7 +16777,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>41365</v>
       </c>
@@ -16901,8 +16797,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="82">
-        <v>42339</v>
+      <c r="A36" s="83">
+        <v>41334</v>
       </c>
       <c r="B36" s="25">
         <v>43.778267</v>
@@ -16919,7 +16815,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>41306</v>
       </c>
@@ -16938,7 +16834,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>41276</v>
       </c>
@@ -16957,7 +16853,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>41246</v>
       </c>
@@ -16977,8 +16873,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="82">
-        <v>42339</v>
+      <c r="A40" s="83">
+        <v>41214</v>
       </c>
       <c r="B40" s="25">
         <v>37.634663000000003</v>
@@ -16995,7 +16891,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>41183</v>
       </c>
@@ -17014,7 +16910,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41156</v>
       </c>
@@ -17033,7 +16929,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41122</v>
       </c>
@@ -17052,7 +16948,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>41092</v>
       </c>
@@ -17071,7 +16967,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>41061</v>
       </c>
@@ -17091,8 +16987,8 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="82">
-        <v>42339</v>
+      <c r="A46" s="83">
+        <v>41030</v>
       </c>
       <c r="B46" s="25">
         <v>29.897804000000001</v>
@@ -17110,8 +17006,8 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="82">
-        <v>42339</v>
+      <c r="A47" s="83">
+        <v>41001</v>
       </c>
       <c r="B47" s="25">
         <v>38.763424000000001</v>
@@ -17128,7 +17024,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>40969</v>
       </c>
@@ -17147,7 +17043,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>40940</v>
       </c>
@@ -17166,7 +17062,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>40911</v>
       </c>
@@ -17185,7 +17081,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>40878</v>
       </c>
@@ -17205,8 +17101,8 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="82">
-        <v>42339</v>
+      <c r="A52" s="83">
+        <v>40848</v>
       </c>
       <c r="B52" s="25">
         <v>27.551694999999999</v>
@@ -17223,7 +17119,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>40819</v>
       </c>
@@ -17243,8 +17139,8 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="82">
-        <v>42339</v>
+      <c r="A54" s="83">
+        <v>40787</v>
       </c>
       <c r="B54" s="25">
         <v>26.561699000000001</v>
@@ -17259,8 +17155,8 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="82">
-        <v>42339</v>
+      <c r="A55" s="83">
+        <v>40756</v>
       </c>
       <c r="B55" s="25">
         <v>33.122757</v>
@@ -17275,8 +17171,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="82">
-        <v>42339</v>
+      <c r="A56" s="83">
+        <v>40725</v>
       </c>
       <c r="B56" s="25">
         <v>35.671337000000001</v>
@@ -17291,8 +17187,8 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="82">
-        <v>42339</v>
+      <c r="A57" s="83">
+        <v>40695</v>
       </c>
       <c r="B57" s="25">
         <v>35.882980000000003</v>
@@ -17307,8 +17203,8 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="82">
-        <v>42339</v>
+      <c r="A58" s="83">
+        <v>40665</v>
       </c>
       <c r="B58" s="25">
         <v>37.898884000000002</v>
@@ -17323,8 +17219,8 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="82">
-        <v>42339</v>
+      <c r="A59" s="83">
+        <v>40634</v>
       </c>
       <c r="B59" s="25">
         <v>39.993664000000003</v>
@@ -17339,8 +17235,8 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="82">
-        <v>42339</v>
+      <c r="A60" s="83">
+        <v>40603</v>
       </c>
       <c r="B60" s="25">
         <v>40.187668000000002</v>
@@ -17354,7 +17250,7 @@
         <v>0.98736347108250222</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>40575</v>
       </c>
@@ -17370,7 +17266,7 @@
         <v>1.0389408306835048</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>40546</v>
       </c>
@@ -17386,7 +17282,7 @@
         <v>1.0606227564286002</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>40513</v>
       </c>
@@ -17403,8 +17299,8 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="82">
-        <v>42339</v>
+      <c r="A64" s="83">
+        <v>40483</v>
       </c>
       <c r="B64" s="25">
         <v>32.566040000000001</v>
@@ -17419,8 +17315,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="82">
-        <v>42339</v>
+      <c r="A65" s="83">
+        <v>40452</v>
       </c>
       <c r="B65" s="25">
         <v>32.766311999999999</v>
@@ -17434,7 +17330,7 @@
         <v>0.98997747238068901</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>40422</v>
       </c>
@@ -17451,8 +17347,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="82">
-        <v>42339</v>
+      <c r="A67" s="83">
+        <v>40392</v>
       </c>
       <c r="B67" s="25">
         <v>31.619671</v>
@@ -17466,7 +17362,7 @@
         <v>0.90268129394800423</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>40360</v>
       </c>
@@ -17483,8 +17379,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="82">
-        <v>42339</v>
+      <c r="A69" s="83">
+        <v>40330</v>
       </c>
       <c r="B69" s="25">
         <v>31.793596000000001</v>
@@ -17499,8 +17395,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="82">
-        <v>42339</v>
+      <c r="A70" s="83">
+        <v>40301</v>
       </c>
       <c r="B70" s="25">
         <v>34.372864</v>
@@ -17515,8 +17411,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="82">
-        <v>42339</v>
+      <c r="A71" s="83">
+        <v>40269</v>
       </c>
       <c r="B71" s="25">
         <v>36.978188000000003</v>
@@ -17530,7 +17426,7 @@
         <v>0.95257286489765725</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>40238</v>
       </c>
@@ -17546,7 +17442,7 @@
         <v>1.0662377263981249</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>40210</v>
       </c>
@@ -17563,8 +17459,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="82">
-        <v>42339</v>
+      <c r="A74" s="83">
+        <v>40182</v>
       </c>
       <c r="B74" s="25">
         <v>33.779274000000001</v>
@@ -17579,8 +17475,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="82">
-        <v>42339</v>
+      <c r="A75" s="83">
+        <v>40148</v>
       </c>
       <c r="B75" s="25">
         <v>36.104095000000001</v>
@@ -17594,7 +17490,7 @@
         <v>0.98070130824297597</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>40119</v>
       </c>
@@ -17611,8 +17507,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="82">
-        <v>42339</v>
+      <c r="A77" s="83">
+        <v>40087</v>
       </c>
       <c r="B77" s="25">
         <v>36.190739000000001</v>
@@ -17626,7 +17522,7 @@
         <v>0.95437115213531121</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>40057</v>
       </c>
@@ -17642,7 +17538,7 @@
         <v>1.0082835203335496</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>40028</v>
       </c>
@@ -17658,7 +17554,7 @@
         <v>1.12445007789934</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>39995</v>
       </c>
@@ -17675,8 +17571,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="82">
-        <v>42339</v>
+      <c r="A81" s="83">
+        <v>39965</v>
       </c>
       <c r="B81" s="25">
         <v>29.474905</v>
@@ -17690,7 +17586,7 @@
         <v>0.92439027679423236</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>39934</v>
       </c>
@@ -17706,7 +17602,7 @@
         <v>1.118181826470702</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>39904</v>
       </c>
@@ -17722,7 +17618,7 @@
         <v>1.243744929629804</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>39874</v>
       </c>
@@ -17739,8 +17635,8 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="82">
-        <v>42339</v>
+      <c r="A85" s="83">
+        <v>39846</v>
       </c>
       <c r="B85" s="25">
         <v>19.709906</v>
@@ -17755,8 +17651,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="82">
-        <v>42339</v>
+      <c r="A86" s="83">
+        <v>39815</v>
       </c>
       <c r="B86" s="25">
         <v>22.004362</v>
@@ -17771,8 +17667,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="82">
-        <v>42339</v>
+      <c r="A87" s="83">
+        <v>39783</v>
       </c>
       <c r="B87" s="25">
         <v>26.869302999999999</v>
@@ -17787,8 +17683,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="82">
-        <v>42339</v>
+      <c r="A88" s="83">
+        <v>39755</v>
       </c>
       <c r="B88" s="25">
         <v>26.980084999999999</v>
@@ -17803,8 +17699,8 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="82">
-        <v>42339</v>
+      <c r="A89" s="83">
+        <v>39722</v>
       </c>
       <c r="B89" s="25">
         <v>35.152512000000002</v>
@@ -17818,7 +17714,7 @@
         <v>0.89011289445927222</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>39693</v>
       </c>
@@ -17835,8 +17731,8 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="82">
-        <v>42339</v>
+      <c r="A91" s="83">
+        <v>39661</v>
       </c>
       <c r="B91" s="25">
         <v>32.549346999999997</v>
@@ -17850,7 +17746,7 @@
         <v>0.9473295176482589</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>39630</v>
       </c>
@@ -17867,8 +17763,8 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="82">
-        <v>42339</v>
+      <c r="A93" s="83">
+        <v>39601</v>
       </c>
       <c r="B93" s="25">
         <v>28.693151</v>
@@ -17883,8 +17779,8 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="82">
-        <v>42339</v>
+      <c r="A94" s="83">
+        <v>39569</v>
       </c>
       <c r="B94" s="25">
         <v>35.960521999999997</v>
@@ -17898,7 +17794,7 @@
         <v>0.90241341141521836</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>39539</v>
       </c>
@@ -17914,7 +17810,7 @@
         <v>1.1184725906091506</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>39510</v>
       </c>
@@ -17931,8 +17827,8 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="82">
-        <v>42339</v>
+      <c r="A97" s="83">
+        <v>39479</v>
       </c>
       <c r="B97" s="25">
         <v>33.720382999999998</v>
@@ -17946,7 +17842,7 @@
         <v>0.85759499320773158</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>39449</v>
       </c>
@@ -17963,24 +17859,24 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="82">
-        <v>42339</v>
+      <c r="A99" s="83">
+        <v>39419</v>
       </c>
       <c r="B99" s="25">
         <v>35.893749</v>
       </c>
       <c r="C99" s="94">
-        <f t="shared" ref="C99:C121" si="6">(B99-B100)/B100</f>
+        <f t="shared" ref="C99:C130" si="6">(B99-B100)/B100</f>
         <v>-4.3182789645221535E-2</v>
       </c>
       <c r="D99" s="8">
-        <f t="shared" ref="D99:D118" si="7">C99+1</f>
+        <f t="shared" ref="D99:D130" si="7">C99+1</f>
         <v>0.95681721035477851</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="82">
-        <v>42339</v>
+      <c r="A100" s="83">
+        <v>39387</v>
       </c>
       <c r="B100" s="25">
         <v>37.513694999999998</v>
@@ -17994,7 +17890,7 @@
         <v>0.97063822660258103</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>39356</v>
       </c>
@@ -18010,7 +17906,7 @@
         <v>1.0340852699246421</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>39329</v>
       </c>
@@ -18026,7 +17922,7 @@
         <v>1.0292003329278443</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>39295</v>
       </c>
@@ -18043,8 +17939,8 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="82">
-        <v>42339</v>
+      <c r="A104" s="83">
+        <v>39265</v>
       </c>
       <c r="B104" s="25">
         <v>35.898173999999997</v>
@@ -18059,8 +17955,8 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="82">
-        <v>42339</v>
+      <c r="A105" s="83">
+        <v>39234</v>
       </c>
       <c r="B105" s="25">
         <v>39.214260000000003</v>
@@ -18075,8 +17971,8 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="82">
-        <v>42339</v>
+      <c r="A106" s="83">
+        <v>39203</v>
       </c>
       <c r="B106" s="25">
         <v>41.949950999999999</v>
@@ -18090,7 +17986,7 @@
         <v>0.99481771692980148</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>39174</v>
       </c>
@@ -18107,8 +18003,8 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="82">
-        <v>42339</v>
+      <c r="A108" s="83">
+        <v>39142</v>
       </c>
       <c r="B108" s="25">
         <v>38.881614999999996</v>
@@ -18123,8 +18019,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="82">
-        <v>42339</v>
+      <c r="A109" s="83">
+        <v>39114</v>
       </c>
       <c r="B109" s="25">
         <v>39.693320999999997</v>
@@ -18138,7 +18034,7 @@
         <v>0.96976236360055612</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>39085</v>
       </c>
@@ -18154,7 +18050,7 @@
         <v>1.0619266709009538</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>39052</v>
       </c>
@@ -18171,8 +18067,8 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="82">
-        <v>42339</v>
+      <c r="A112" s="83">
+        <v>39022</v>
       </c>
       <c r="B112" s="25">
         <v>36.932082999999999</v>
@@ -18186,7 +18082,7 @@
         <v>0.97554803794622924</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>38992</v>
       </c>
@@ -18202,7 +18098,7 @@
         <v>1.0174662652930908</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>38961</v>
       </c>
@@ -18218,7 +18114,7 @@
         <v>1.0284712465643362</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>38930</v>
       </c>
@@ -18234,7 +18130,7 @@
         <v>1.0008768009339852</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>38901</v>
       </c>
@@ -18251,8 +18147,8 @@
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A117" s="82">
-        <v>42339</v>
+      <c r="A117" s="83">
+        <v>38869</v>
       </c>
       <c r="B117" s="25">
         <v>33.008541000000001</v>
@@ -18266,9 +18162,9 @@
         <v>0.98499062770280132</v>
       </c>
     </row>
-    <row r="118" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="82">
-        <v>42339</v>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A118" s="83">
+        <v>38838</v>
       </c>
       <c r="B118" s="25">
         <v>33.511527999999998</v>
@@ -18282,9 +18178,9 @@
         <v>0.93962093421484139</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A119" s="82">
-        <v>42339</v>
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>38810</v>
       </c>
       <c r="B119">
         <v>35.664943999999998</v>
@@ -18298,9 +18194,9 @@
         <v>1.0987268211483416</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A120" s="82">
-        <v>42339</v>
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>38777</v>
       </c>
       <c r="B120">
         <v>32.460247000000003</v>
@@ -18314,9 +18210,9 @@
         <v>1.0121536716967037</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A121" s="82">
-        <v>42339</v>
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>38749</v>
       </c>
       <c r="B121">
         <v>32.070473</v>
@@ -18331,8 +18227,8 @@
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A122" s="82">
-        <v>42339</v>
+      <c r="A122" s="84">
+        <v>38720</v>
       </c>
       <c r="B122" s="81">
         <v>30.986908</v>
@@ -18760,27 +18656,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113" t="s">
+      <c r="B1" s="98"/>
+      <c r="C1" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="113"/>
+      <c r="D1" s="98"/>
       <c r="E1" s="79" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="33"/>
-      <c r="G1" s="111" t="s">
+      <c r="G1" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="112"/>
+      <c r="H1" s="97"/>
       <c r="I1" s="33"/>
-      <c r="J1" s="111" t="s">
+      <c r="J1" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="112"/>
+      <c r="K1" s="97"/>
       <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18892,10 +18788,10 @@
         <v>42</v>
       </c>
       <c r="I5" s="34"/>
-      <c r="J5" s="116" t="s">
+      <c r="J5" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="117"/>
+      <c r="K5" s="102"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="83">
@@ -20535,11 +20431,11 @@
         <v>28.942726</v>
       </c>
       <c r="C99" s="45">
-        <f t="shared" ref="C99:C121" si="6">(B99-B100)/B100</f>
+        <f t="shared" ref="C99:C130" si="6">(B99-B100)/B100</f>
         <v>5.9523854411705067E-2</v>
       </c>
       <c r="D99" s="20">
-        <f t="shared" ref="D99:D121" si="7">1+C99</f>
+        <f t="shared" ref="D99:D130" si="7">1+C99</f>
         <v>1.0595238544117052</v>
       </c>
     </row>
@@ -21245,10 +21141,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="113"/>
+      <c r="B1" s="98"/>
       <c r="C1" s="35" t="s">
         <v>7</v>
       </c>
@@ -21257,14 +21153,14 @@
         <v>8</v>
       </c>
       <c r="F1" s="33"/>
-      <c r="G1" s="111" t="s">
+      <c r="G1" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="112"/>
-      <c r="J1" s="116" t="s">
+      <c r="H1" s="97"/>
+      <c r="J1" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="117"/>
+      <c r="K1" s="102"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
@@ -21375,10 +21271,10 @@
       <c r="H5" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="118" t="s">
+      <c r="J5" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="119"/>
+      <c r="K5" s="104"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="83">
@@ -22991,11 +22887,11 @@
         <v>16.068100000000001</v>
       </c>
       <c r="C99" s="45">
-        <f t="shared" ref="C99:C121" si="6">(B99-B100)/B100</f>
+        <f t="shared" ref="C99:C130" si="6">(B99-B100)/B100</f>
         <v>-4.335028694847478E-2</v>
       </c>
       <c r="D99" s="8">
-        <f t="shared" ref="D99:D121" si="7">1+C99</f>
+        <f t="shared" ref="D99:D130" si="7">1+C99</f>
         <v>0.95664971305152524</v>
       </c>
     </row>
@@ -23806,22 +23702,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="123" t="s">
+      <c r="B1" s="106"/>
+      <c r="C1" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="124"/>
+      <c r="D1" s="109"/>
       <c r="E1" s="51" t="s">
         <v>53</v>
       </c>
       <c r="F1" s="58"/>
-      <c r="G1" s="122" t="s">
+      <c r="G1" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="122"/>
+      <c r="H1" s="107"/>
       <c r="I1" s="54"/>
       <c r="J1" s="36" t="s">
         <v>50</v>
@@ -23938,10 +23834,10 @@
         <v>42</v>
       </c>
       <c r="I5" s="54"/>
-      <c r="J5" s="122" t="s">
+      <c r="J5" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="122"/>
+      <c r="K5" s="107"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="41">
@@ -25640,11 +25536,11 @@
         <v>98.306297000000001</v>
       </c>
       <c r="C99" s="45">
-        <f t="shared" ref="C99:C121" si="6">(B99-B100)/B100</f>
+        <f t="shared" ref="C99:C130" si="6">(B99-B100)/B100</f>
         <v>0.12398115148323133</v>
       </c>
       <c r="D99" s="20">
-        <f t="shared" ref="D99:D121" si="7">1+C99</f>
+        <f t="shared" ref="D99:D130" si="7">1+C99</f>
         <v>1.1239811514832314</v>
       </c>
     </row>

</xml_diff>